<commit_message>
Started work on the group B rubric
</commit_message>
<xml_diff>
--- a/labs/Lab01/CS133JS_Lab01_Rubrics.xlsx
+++ b/labs/Lab01/CS133JS_Lab01_Rubrics.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/birdb/Projects/CS133JS-CourseMaterials/labs/Lab01/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44AB8AF1-8215-7846-82F9-2CC6FD21071F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE4A71B4-2DCA-6846-A655-E85747D2D417}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13060" yWindow="5200" windowWidth="28040" windowHeight="17440" xr2:uid="{9702CE45-50CE-F14F-802C-E5FE921247A2}"/>
+    <workbookView xWindow="13060" yWindow="5200" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{9702CE45-50CE-F14F-802C-E5FE921247A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Group A" sheetId="1" r:id="rId1"/>
+    <sheet name="Group B" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>Criteria</t>
   </si>
@@ -67,6 +68,30 @@
   </si>
   <si>
     <t>Caption using variable and document.write</t>
+  </si>
+  <si>
+    <t>Are the correct developer’s name and date in a comment in the head element of the HTML page?</t>
+  </si>
+  <si>
+    <t>Is a variable used for the favorite site name?</t>
+  </si>
+  <si>
+    <t>Is a variable used for the site URL?</t>
+  </si>
+  <si>
+    <t>Is the HTML that displays the link to the web site produced by a document.write statement?</t>
+  </si>
+  <si>
+    <t>Is the caption produced by a document.write statement?</t>
+  </si>
+  <si>
+    <t>Is a heading displayed for the page?</t>
+  </si>
+  <si>
+    <t>Is the link displayed correctly?</t>
+  </si>
+  <si>
+    <t>Assignment Group B – Favorite web site</t>
   </si>
 </sst>
 </file>
@@ -438,7 +463,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3216228F-B421-8943-9C69-C9FAC1E7C520}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -554,4 +579,108 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D6A7069-CD8C-C44F-B7C6-148A7A61DB13}">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12">
+        <f>SUM(D4:D10)</f>
+        <v>40</v>
+      </c>
+      <c r="E12">
+        <f>SUM(E4:E10)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>